<commit_message>
Updated Drug NDC fields docs.
</commit_message>
<xml_diff>
--- a/static/fields/drugndc_reference.xlsx
+++ b/static/fields/drugndc_reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackfinch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.finch/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B763F1C-F5C8-434B-B97B-2B15D7E6AC1E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7303886-790C-DE4D-909B-56B033F1E216}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="760" windowWidth="26540" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,109 +156,109 @@
     <t>dea_schedule</t>
   </si>
   <si>
+    <t>listing_expiration_date</t>
+  </si>
+  <si>
+    <t>This is the date when the listing record will expire if not updated or certified by the firm.</t>
+  </si>
+  <si>
+    <t>packaging</t>
+  </si>
+  <si>
+    <t>package_ndc</t>
+  </si>
+  <si>
+    <t>This number, known as the NDC, identifies the labeler, product, and trade package size. The first segment, the labeler code, is assigned by the FDA. A labeler is any firm that manufactures (including repackers or relabelers), or distributes (under its own name) the drug.</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>A description of the size and type of packaging in sentence form. Multilevel packages will have the descriptions concatenated together.</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>Indicates whether this is a sample packaging or not.</t>
+  </si>
+  <si>
+    <t>openfda</t>
+  </si>
+  <si>
+    <t>is_original_packager</t>
+  </si>
+  <si>
+    <t>Whether or not the drug has been repackaged for distribution.</t>
+  </si>
+  <si>
+    <t>manufacturer_name</t>
+  </si>
+  <si>
+    <t>Name of manufacturer or company that makes this drug product, corresponding to the labeler code segment of the NDC.</t>
+  </si>
+  <si>
+    <t>Unique identifier applied to a drug concept within the National Drug File Reference Terminology (NDF-RT).</t>
+  </si>
+  <si>
+    <t>nui</t>
+  </si>
+  <si>
+    <t>pharm_class_cs</t>
+  </si>
+  <si>
+    <t>Chemical structure classification of the drug product’s pharmacologic class. Takes the form of the classification, followed by `[Chemical/Ingredient]` (such as `Thiazides [Chemical/Ingredient]` or `Antibodies, Monoclonal [Chemical/Ingredient].</t>
+  </si>
+  <si>
+    <t>pharm_class_epc</t>
+  </si>
+  <si>
+    <t>pharm_class_moa</t>
+  </si>
+  <si>
+    <t>pharm_class_pe</t>
+  </si>
+  <si>
+    <t>rxcui</t>
+  </si>
+  <si>
+    <t>spl_set_id</t>
+  </si>
+  <si>
+    <t>unii</t>
+  </si>
+  <si>
+    <t>upc</t>
+  </si>
+  <si>
+    <t>Established pharmacologic class associated with an approved indication of an active moiety (generic drug) that the FDA has determined to be scientifically valid and clinically meaningful. Takes the form of the pharmacologic class, followed by `[EPC]` (such as `Thiazide Diuretic [EPC]` or `Tumor Necrosis Factor Blocker [EPC]`.</t>
+  </si>
+  <si>
+    <t>Mechanism of action of the drug—molecular, subcellular, or cellular functional activity—of the drug’s established pharmacologic class. Takes the form of the mechanism of action, followed by `[MoA]` (such as `Calcium Channel Antagonists [MoA]` or `Tumor Necrosis Factor Receptor Blocking Activity [MoA]`.</t>
+  </si>
+  <si>
+    <t>Physiologic effect or pharmacodynamic effect—tissue, organ, or organ system level functional activity—of the drug’s established pharmacologic class. Takes the form of the effect, followed by `[PE]` (such as `Increased Diuresis [PE]` or `Decreased Cytokine Activity [PE]`.</t>
+  </si>
+  <si>
+    <t>The RxNorm Concept Unique Identifier. RxCUI is a unique number that describes a semantic concept about the drug product, including its ingredients, strength, and dose forms.</t>
+  </si>
+  <si>
+    <t>Unique identifier for the Structured Product Label for a product, which is stable across versions of the label. Also referred to as the set ID.</t>
+  </si>
+  <si>
+    <t>Unique Ingredient Identifier, which is a non-proprietary, free, unique, unambiguous, non-semantic, alphanumeric identifier based on a substance’s molecular structure and/or descriptive information.</t>
+  </si>
+  <si>
+    <t>Universal Product Code</t>
+  </si>
+  <si>
     <t>This is the assigned DEA Schedule number as reported by the labeler. Values are CI, CII, CIII, CIV, and CV.
 Value is one of the following
-1 = ci
-2 = cii
-3 = cii
-4 = civ
-5 = cv</t>
-  </si>
-  <si>
-    <t>listing_expiration_date</t>
-  </si>
-  <si>
-    <t>This is the date when the listing record will expire if not updated or certified by the firm.</t>
-  </si>
-  <si>
-    <t>packaging</t>
-  </si>
-  <si>
-    <t>package_ndc</t>
-  </si>
-  <si>
-    <t>This number, known as the NDC, identifies the labeler, product, and trade package size. The first segment, the labeler code, is assigned by the FDA. A labeler is any firm that manufactures (including repackers or relabelers), or distributes (under its own name) the drug.</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>A description of the size and type of packaging in sentence form. Multilevel packages will have the descriptions concatenated together.</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>Indicates whether this is a sample packaging or not.</t>
-  </si>
-  <si>
-    <t>openfda</t>
-  </si>
-  <si>
-    <t>is_original_packager</t>
-  </si>
-  <si>
-    <t>Whether or not the drug has been repackaged for distribution.</t>
-  </si>
-  <si>
-    <t>manufacturer_name</t>
-  </si>
-  <si>
-    <t>Name of manufacturer or company that makes this drug product, corresponding to the labeler code segment of the NDC.</t>
-  </si>
-  <si>
-    <t>Unique identifier applied to a drug concept within the National Drug File Reference Terminology (NDF-RT).</t>
-  </si>
-  <si>
-    <t>nui</t>
-  </si>
-  <si>
-    <t>pharm_class_cs</t>
-  </si>
-  <si>
-    <t>Chemical structure classification of the drug product’s pharmacologic class. Takes the form of the classification, followed by `[Chemical/Ingredient]` (such as `Thiazides [Chemical/Ingredient]` or `Antibodies, Monoclonal [Chemical/Ingredient].</t>
-  </si>
-  <si>
-    <t>pharm_class_epc</t>
-  </si>
-  <si>
-    <t>pharm_class_moa</t>
-  </si>
-  <si>
-    <t>pharm_class_pe</t>
-  </si>
-  <si>
-    <t>rxcui</t>
-  </si>
-  <si>
-    <t>spl_set_id</t>
-  </si>
-  <si>
-    <t>unii</t>
-  </si>
-  <si>
-    <t>upc</t>
-  </si>
-  <si>
-    <t>Established pharmacologic class associated with an approved indication of an active moiety (generic drug) that the FDA has determined to be scientifically valid and clinically meaningful. Takes the form of the pharmacologic class, followed by `[EPC]` (such as `Thiazide Diuretic [EPC]` or `Tumor Necrosis Factor Blocker [EPC]`.</t>
-  </si>
-  <si>
-    <t>Mechanism of action of the drug—molecular, subcellular, or cellular functional activity—of the drug’s established pharmacologic class. Takes the form of the mechanism of action, followed by `[MoA]` (such as `Calcium Channel Antagonists [MoA]` or `Tumor Necrosis Factor Receptor Blocking Activity [MoA]`.</t>
-  </si>
-  <si>
-    <t>Physiologic effect or pharmacodynamic effect—tissue, organ, or organ system level functional activity—of the drug’s established pharmacologic class. Takes the form of the effect, followed by `[PE]` (such as `Increased Diuresis [PE]` or `Decreased Cytokine Activity [PE]`.</t>
-  </si>
-  <si>
-    <t>The RxNorm Concept Unique Identifier. RxCUI is a unique number that describes a semantic concept about the drug product, including its ingredients, strength, and dose forms.</t>
-  </si>
-  <si>
-    <t>Unique identifier for the Structured Product Label for a product, which is stable across versions of the label. Also referred to as the set ID.</t>
-  </si>
-  <si>
-    <t>Unique Ingredient Identifier, which is a non-proprietary, free, unique, unambiguous, non-semantic, alphanumeric identifier based on a substance’s molecular structure and/or descriptive information.</t>
-  </si>
-  <si>
-    <t>Universal Product Code</t>
+1 = CI
+2 = CII
+3 = CIII
+4 = CIV
+5 = CV</t>
   </si>
 </sst>
 </file>
@@ -1116,8 +1116,8 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
@@ -1309,97 +1309,97 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B20" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>27</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>29</v>
@@ -1427,170 +1427,170 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="C37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>